<commit_message>
diagramme de classes et orth dico+mcd
</commit_message>
<xml_diff>
--- a/Stage/Dictionnaire de donnée.xlsx
+++ b/Stage/Dictionnaire de donnée.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\59011-07-07\CDA_nils\Stage\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -222,9 +227,6 @@
     <t>permet en dehors de l'application d'identifier une formation</t>
   </si>
   <si>
-    <t>distancielsReccurents</t>
-  </si>
-  <si>
     <t>l'id de l'action auquel la journée de distanciel est rataché</t>
   </si>
   <si>
@@ -237,21 +239,12 @@
     <t>idJour</t>
   </si>
   <si>
-    <t>idDistancielReccurent</t>
-  </si>
-  <si>
     <t>le numero du jour de la semaine en distanciel</t>
   </si>
   <si>
     <t>numéro unique utilisé seulement par l'application pour identifier ce distanciel</t>
   </si>
   <si>
-    <t>distancielsPresentielsExeptionels</t>
-  </si>
-  <si>
-    <t>idDistancielPresentielExeptionel</t>
-  </si>
-  <si>
     <t>distanciel ou presentiel</t>
   </si>
   <si>
@@ -459,18 +452,12 @@
     <t>numéro unique utilisé seulement par l'application pour identifier un utilisateur</t>
   </si>
   <si>
-    <t>Ratachements</t>
-  </si>
-  <si>
     <t>id du centre</t>
   </si>
   <si>
     <t>id de l'utilisateur</t>
   </si>
   <si>
-    <t>idRatachement</t>
-  </si>
-  <si>
     <t>numéro unique utilisé seulement par l'application pour identifier le lien entre un employer et un site</t>
   </si>
   <si>
@@ -583,13 +570,31 @@
   </si>
   <si>
     <t>l'id du centre d'origine de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Rattachements</t>
+  </si>
+  <si>
+    <t>idRattachement</t>
+  </si>
+  <si>
+    <t>distancielsPresentielsExceptionnels</t>
+  </si>
+  <si>
+    <t>idDPE</t>
+  </si>
+  <si>
+    <t>idDR</t>
+  </si>
+  <si>
+    <t>distancielsRecurrents</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -811,19 +816,28 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -859,28 +873,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -889,6 +894,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -935,7 +948,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -967,9 +980,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1001,6 +1015,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1176,14 +1191,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38" customWidth="1"/>
     <col min="3" max="3" width="36.5703125" customWidth="1"/>
@@ -1194,8 +1209,8 @@
     <col min="8" max="8" width="126.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
@@ -1218,7 +1233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1">
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1227,9 +1242,9 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="49" t="s">
-        <v>112</v>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="56" t="s">
+        <v>108</v>
       </c>
       <c r="C4" s="36" t="s">
         <v>24</v>
@@ -1245,29 +1260,29 @@
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="37" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B5" s="50"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="57"/>
       <c r="C5" s="38" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F5" s="38" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="38"/>
       <c r="H5" s="39" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1276,8 +1291,8 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="2:8">
-      <c r="B7" s="46" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="53" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1297,8 +1312,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
-      <c r="B8" s="47"/>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="54"/>
       <c r="C8" s="4" t="s">
         <v>59</v>
       </c>
@@ -1316,8 +1331,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
-      <c r="B9" s="47"/>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="54"/>
       <c r="C9" s="4" t="s">
         <v>60</v>
       </c>
@@ -1335,8 +1350,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B10" s="48"/>
+    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="55"/>
       <c r="C10" s="6" t="s">
         <v>51</v>
       </c>
@@ -1352,9 +1367,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="12" spans="2:8">
-      <c r="B12" s="57" t="s">
+    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="50" t="s">
         <v>46</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -1374,8 +1389,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
-      <c r="B13" s="58"/>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="51"/>
       <c r="C13" s="10" t="s">
         <v>9</v>
       </c>
@@ -1393,8 +1408,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
-      <c r="B14" s="58"/>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="51"/>
       <c r="C14" s="10" t="s">
         <v>13</v>
       </c>
@@ -1410,8 +1425,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
-      <c r="B15" s="58"/>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="51"/>
       <c r="C15" s="10" t="s">
         <v>17</v>
       </c>
@@ -1427,8 +1442,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
-      <c r="B16" s="58"/>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="51"/>
       <c r="C16" s="10" t="s">
         <v>21</v>
       </c>
@@ -1444,27 +1459,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="58"/>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="51"/>
       <c r="C17" s="10" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="58"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="51"/>
       <c r="C18" s="10" t="s">
         <v>25</v>
       </c>
@@ -1480,8 +1495,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
-      <c r="B19" s="58"/>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="51"/>
       <c r="C19" s="10" t="s">
         <v>29</v>
       </c>
@@ -1499,8 +1514,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="58"/>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="51"/>
       <c r="C20" s="10" t="s">
         <v>31</v>
       </c>
@@ -1518,8 +1533,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="58"/>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="51"/>
       <c r="C21" s="10" t="s">
         <v>53</v>
       </c>
@@ -1537,8 +1552,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B22" s="59"/>
+    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="52"/>
       <c r="C22" s="12" t="s">
         <v>54</v>
       </c>
@@ -1556,9 +1571,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="24" spans="2:8">
-      <c r="B24" s="46" t="s">
+    <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="53" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1578,8 +1593,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="2:8">
-      <c r="B25" s="47"/>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="54"/>
       <c r="C25" s="4" t="s">
         <v>13</v>
       </c>
@@ -1595,8 +1610,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="2:8">
-      <c r="B26" s="47"/>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="54"/>
       <c r="C26" s="4" t="s">
         <v>17</v>
       </c>
@@ -1612,8 +1627,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B27" s="48"/>
+    <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="55"/>
       <c r="C27" s="6" t="s">
         <v>37</v>
       </c>
@@ -1631,9 +1646,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="29" spans="2:8">
-      <c r="B29" s="46" t="s">
+    <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="53" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1653,8 +1668,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="2:8">
-      <c r="B30" s="47"/>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="54"/>
       <c r="C30" s="4" t="s">
         <v>13</v>
       </c>
@@ -1670,10 +1685,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="2:8">
-      <c r="B31" s="47"/>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="54"/>
       <c r="C31" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>48</v>
@@ -1687,8 +1702,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B32" s="48"/>
+    <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="55"/>
       <c r="C32" s="6" t="s">
         <v>37</v>
       </c>
@@ -1706,16 +1721,16 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="34" spans="2:8">
-      <c r="B34" s="46" t="s">
-        <v>68</v>
+    <row r="33" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="53" t="s">
+        <v>188</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>73</v>
+        <v>187</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>19</v>
@@ -1725,30 +1740,30 @@
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8">
-      <c r="B35" s="47"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="54"/>
       <c r="C35" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B36" s="48"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="55"/>
       <c r="C36" s="6" t="s">
         <v>37</v>
       </c>
@@ -1763,19 +1778,19 @@
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="38" spans="2:8">
-      <c r="B38" s="46" t="s">
-        <v>76</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="53" t="s">
+        <v>185</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>77</v>
+        <v>186</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>19</v>
@@ -1785,30 +1800,30 @@
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8">
-      <c r="B39" s="47"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="54"/>
       <c r="C39" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8">
-      <c r="B40" s="47"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="54"/>
       <c r="C40" s="4" t="s">
         <v>13</v>
       </c>
@@ -1821,13 +1836,13 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8">
-      <c r="B41" s="47"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="54"/>
       <c r="C41" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>48</v>
@@ -1838,11 +1853,11 @@
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B42" s="48"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="55"/>
       <c r="C42" s="6" t="s">
         <v>37</v>
       </c>
@@ -1857,19 +1872,19 @@
       </c>
       <c r="G42" s="6"/>
       <c r="H42" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="44" spans="2:8">
-      <c r="B44" s="46" t="s">
-        <v>88</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="53" t="s">
+        <v>84</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>19</v>
@@ -1879,16 +1894,16 @@
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8">
-      <c r="B45" s="47"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="54"/>
       <c r="C45" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>15</v>
@@ -1896,16 +1911,16 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8">
-      <c r="B46" s="47"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="54"/>
       <c r="C46" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>19</v>
@@ -1915,16 +1930,16 @@
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8">
-      <c r="B47" s="47"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="54"/>
       <c r="C47" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>19</v>
@@ -1934,11 +1949,11 @@
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B48" s="48"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="55"/>
       <c r="C48" s="6" t="s">
         <v>37</v>
       </c>
@@ -1953,19 +1968,19 @@
       </c>
       <c r="G48" s="6"/>
       <c r="H48" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="50" spans="2:8">
-      <c r="B50" s="46" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="53" t="s">
+        <v>96</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>19</v>
@@ -1975,35 +1990,35 @@
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8">
-      <c r="B51" s="47"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="54"/>
       <c r="C51" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8">
-      <c r="B52" s="47"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="54"/>
       <c r="C52" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>19</v>
@@ -2013,16 +2028,16 @@
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8">
-      <c r="B53" s="47"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="54"/>
       <c r="C53" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>19</v>
@@ -2032,11 +2047,11 @@
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B54" s="48"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="55"/>
       <c r="C54" s="6" t="s">
         <v>37</v>
       </c>
@@ -2051,19 +2066,19 @@
       </c>
       <c r="G54" s="6"/>
       <c r="H54" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="56" spans="2:8">
-      <c r="B56" s="51" t="s">
-        <v>117</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="58" t="s">
+        <v>113</v>
       </c>
       <c r="C56" s="30" t="s">
         <v>24</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E56" s="30" t="s">
         <v>19</v>
@@ -2073,28 +2088,28 @@
       </c>
       <c r="G56" s="30"/>
       <c r="H56" s="31" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8">
-      <c r="B57" s="52"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="59"/>
       <c r="C57" s="32" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E57" s="32" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F57" s="32"/>
       <c r="G57" s="32"/>
       <c r="H57" s="33" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B58" s="53"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="60"/>
       <c r="C58" s="34" t="s">
         <v>53</v>
       </c>
@@ -2109,19 +2124,19 @@
       </c>
       <c r="G58" s="34"/>
       <c r="H58" s="35" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="60" spans="2:8">
-      <c r="B60" s="54" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="61" t="s">
+        <v>119</v>
       </c>
       <c r="C60" s="24" t="s">
         <v>24</v>
       </c>
       <c r="D60" s="24" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E60" s="24" t="s">
         <v>19</v>
@@ -2131,16 +2146,16 @@
       </c>
       <c r="G60" s="24"/>
       <c r="H60" s="25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8">
-      <c r="B61" s="55"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="62"/>
       <c r="C61" s="26" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D61" s="26" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E61" s="26" t="s">
         <v>19</v>
@@ -2150,13 +2165,13 @@
       </c>
       <c r="G61" s="26"/>
       <c r="H61" s="27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8">
-      <c r="B62" s="55"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="62"/>
       <c r="C62" s="26" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D62" s="26" t="s">
         <v>7</v>
@@ -2169,11 +2184,11 @@
       </c>
       <c r="G62" s="26"/>
       <c r="H62" s="27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8">
-      <c r="B63" s="55"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="62"/>
       <c r="C63" s="26" t="s">
         <v>13</v>
       </c>
@@ -2186,13 +2201,13 @@
       <c r="F63" s="26"/>
       <c r="G63" s="26"/>
       <c r="H63" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B64" s="56"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="63"/>
       <c r="C64" s="28" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D64" s="28" t="s">
         <v>48</v>
@@ -2203,164 +2218,164 @@
       <c r="F64" s="28"/>
       <c r="G64" s="28"/>
       <c r="H64" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="E66" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F66" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="G66" s="41"/>
+      <c r="H66" s="42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="48"/>
+      <c r="C67" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D67" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="E67" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" s="43"/>
+      <c r="H67" s="44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="48"/>
+      <c r="C68" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="D68" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="E68" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="F68" s="43"/>
+      <c r="G68" s="43"/>
+      <c r="H68" s="44"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="48"/>
+      <c r="C69" s="43" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="65" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="66" spans="2:8">
-      <c r="B66" s="60" t="s">
+      <c r="D69" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="E69" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="F69" s="43"/>
+      <c r="G69" s="43"/>
+      <c r="H69" s="44"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="48"/>
+      <c r="C70" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="D70" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="C66" s="61" t="s">
-        <v>24</v>
-      </c>
-      <c r="D66" s="61" t="s">
+      <c r="E70" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="F70" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="G70" s="43"/>
+      <c r="H70" s="44" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="48"/>
+      <c r="C71" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="E71" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="F71" s="43"/>
+      <c r="G71" s="43"/>
+      <c r="H71" s="44" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="48"/>
+      <c r="C72" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="D72" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="E72" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F72" s="43"/>
+      <c r="G72" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="H72" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="E66" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="F66" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="G66" s="61"/>
-      <c r="H66" s="62" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8">
-      <c r="B67" s="63"/>
-      <c r="C67" s="64" t="s">
-        <v>132</v>
-      </c>
-      <c r="D67" s="64" t="s">
-        <v>132</v>
-      </c>
-      <c r="E67" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="F67" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="G67" s="64"/>
-      <c r="H67" s="65" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8">
-      <c r="B68" s="63"/>
-      <c r="C68" s="64" t="s">
-        <v>133</v>
-      </c>
-      <c r="D68" s="64" t="s">
-        <v>133</v>
-      </c>
-      <c r="E68" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="F68" s="64"/>
-      <c r="G68" s="64"/>
-      <c r="H68" s="65"/>
-    </row>
-    <row r="69" spans="2:8">
-      <c r="B69" s="63"/>
-      <c r="C69" s="64" t="s">
-        <v>134</v>
-      </c>
-      <c r="D69" s="64" t="s">
-        <v>134</v>
-      </c>
-      <c r="E69" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="F69" s="64"/>
-      <c r="G69" s="64"/>
-      <c r="H69" s="65"/>
-    </row>
-    <row r="70" spans="2:8">
-      <c r="B70" s="63"/>
-      <c r="C70" s="64" t="s">
-        <v>142</v>
-      </c>
-      <c r="D70" s="64" t="s">
-        <v>135</v>
-      </c>
-      <c r="E70" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="F70" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="G70" s="64"/>
-      <c r="H70" s="65" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8">
-      <c r="B71" s="63"/>
-      <c r="C71" s="64" t="s">
-        <v>141</v>
-      </c>
-      <c r="D71" s="64" t="s">
-        <v>136</v>
-      </c>
-      <c r="E71" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="F71" s="64"/>
-      <c r="G71" s="64"/>
-      <c r="H71" s="65" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="72" spans="2:8">
-      <c r="B72" s="63"/>
-      <c r="C72" s="64" t="s">
-        <v>137</v>
-      </c>
-      <c r="D72" s="64" t="s">
-        <v>137</v>
-      </c>
-      <c r="E72" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="F72" s="64"/>
-      <c r="G72" s="64" t="s">
+    </row>
+    <row r="73" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="49"/>
+      <c r="C73" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="H72" s="65" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B73" s="68"/>
-      <c r="C73" s="66" t="s">
-        <v>148</v>
-      </c>
-      <c r="D73" s="66" t="s">
+      <c r="D73" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="E73" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="F73" s="66" t="s">
+      <c r="E73" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F73" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="G73" s="66"/>
-      <c r="H73" s="67" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="75" spans="2:8">
-      <c r="B75" s="41" t="s">
-        <v>147</v>
+      <c r="G73" s="45"/>
+      <c r="H73" s="46" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="64" t="s">
+        <v>183</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
       <c r="E75" s="14" t="s">
         <v>19</v>
@@ -2370,13 +2385,13 @@
       </c>
       <c r="G75" s="14"/>
       <c r="H75" s="15" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="76" spans="2:8">
-      <c r="B76" s="42"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="65"/>
       <c r="C76" s="16" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D76" s="16" t="s">
         <v>55</v>
@@ -2389,16 +2404,16 @@
       </c>
       <c r="G76" s="16"/>
       <c r="H76" s="17" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B77" s="43"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="66"/>
       <c r="C77" s="18" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E77" s="18" t="s">
         <v>19</v>
@@ -2408,19 +2423,19 @@
       </c>
       <c r="G77" s="18"/>
       <c r="H77" s="19" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="79" spans="2:8">
-      <c r="B79" s="41" t="s">
-        <v>154</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="64" t="s">
+        <v>148</v>
       </c>
       <c r="C79" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E79" s="14" t="s">
         <v>19</v>
@@ -2430,16 +2445,16 @@
       </c>
       <c r="G79" s="14"/>
       <c r="H79" s="15" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="80" spans="2:8">
-      <c r="B80" s="42"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="65"/>
       <c r="C80" s="16" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D80" s="16" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E80" s="16" t="s">
         <v>19</v>
@@ -2449,13 +2464,13 @@
       </c>
       <c r="G80" s="16"/>
       <c r="H80" s="17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="81" spans="2:8">
-      <c r="B81" s="42"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="65"/>
       <c r="C81" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D81" s="16" t="s">
         <v>7</v>
@@ -2468,11 +2483,11 @@
       </c>
       <c r="G81" s="16"/>
       <c r="H81" s="17" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8">
-      <c r="B82" s="42"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="65"/>
       <c r="C82" s="16" t="s">
         <v>13</v>
       </c>
@@ -2485,13 +2500,13 @@
       <c r="F82" s="16"/>
       <c r="G82" s="16"/>
       <c r="H82" s="17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B83" s="43"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="66"/>
       <c r="C83" s="18" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D83" s="18" t="s">
         <v>48</v>
@@ -2502,19 +2517,19 @@
       <c r="F83" s="18"/>
       <c r="G83" s="18"/>
       <c r="H83" s="19" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="85" spans="2:8">
-      <c r="B85" s="41" t="s">
-        <v>161</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="64" t="s">
+        <v>155</v>
       </c>
       <c r="C85" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E85" s="14" t="s">
         <v>19</v>
@@ -2524,30 +2539,30 @@
       </c>
       <c r="G85" s="14"/>
       <c r="H85" s="15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8">
-      <c r="B86" s="42"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="65"/>
       <c r="C86" s="16" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D86" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E86" s="16" t="s">
         <v>19</v>
       </c>
       <c r="F86" s="16"/>
       <c r="G86" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H86" s="17" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8">
-      <c r="B87" s="42"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="65"/>
       <c r="C87" s="16" t="s">
         <v>13</v>
       </c>
@@ -2560,13 +2575,13 @@
       <c r="F87" s="16"/>
       <c r="G87" s="16"/>
       <c r="H87" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="88" spans="2:8">
-      <c r="B88" s="42"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="65"/>
       <c r="C88" s="16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D88" s="16" t="s">
         <v>48</v>
@@ -2579,16 +2594,16 @@
       </c>
       <c r="G88" s="16"/>
       <c r="H88" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="89" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B89" s="43"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="66"/>
       <c r="C89" s="18" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E89" s="18" t="s">
         <v>19</v>
@@ -2598,19 +2613,19 @@
       </c>
       <c r="G89" s="18"/>
       <c r="H89" s="19" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="90" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="91" spans="2:8">
-      <c r="B91" s="44" t="s">
-        <v>171</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="67" t="s">
+        <v>165</v>
       </c>
       <c r="C91" s="20" t="s">
         <v>24</v>
       </c>
       <c r="D91" s="20" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E91" s="20" t="s">
         <v>19</v>
@@ -2620,38 +2635,38 @@
       </c>
       <c r="G91" s="20"/>
       <c r="H91" s="21" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="92" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B92" s="45"/>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="68"/>
       <c r="C92" s="22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D92" s="22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E92" s="22" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F92" s="22" t="s">
         <v>11</v>
       </c>
       <c r="G92" s="22"/>
       <c r="H92" s="23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="93" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="94" spans="2:8">
-      <c r="B94" s="41" t="s">
-        <v>176</v>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="64" t="s">
+        <v>170</v>
       </c>
       <c r="C94" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E94" s="14" t="s">
         <v>19</v>
@@ -2661,16 +2676,16 @@
       </c>
       <c r="G94" s="14"/>
       <c r="H94" s="15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="95" spans="2:8">
-      <c r="B95" s="42"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="65"/>
       <c r="C95" s="16" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D95" s="16" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E95" s="16" t="s">
         <v>19</v>
@@ -2680,16 +2695,16 @@
       </c>
       <c r="G95" s="16"/>
       <c r="H95" s="17" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="96" spans="2:8">
-      <c r="B96" s="42"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B96" s="65"/>
       <c r="C96" s="16" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E96" s="16" t="s">
         <v>19</v>
@@ -2699,13 +2714,13 @@
       </c>
       <c r="G96" s="16"/>
       <c r="H96" s="17" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="97" spans="2:8">
-      <c r="B97" s="42"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="65"/>
       <c r="C97" s="16" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D97" s="16" t="s">
         <v>14</v>
@@ -2716,13 +2731,13 @@
       <c r="F97" s="16"/>
       <c r="G97" s="16"/>
       <c r="H97" s="17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="98" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B98" s="43"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="66"/>
       <c r="C98" s="18" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D98" s="18" t="s">
         <v>48</v>
@@ -2735,11 +2750,19 @@
       </c>
       <c r="G98" s="18"/>
       <c r="H98" s="19" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B85:B89"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="B94:B98"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="B60:B64"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B79:B83"/>
     <mergeCell ref="B66:B73"/>
     <mergeCell ref="B12:B22"/>
     <mergeCell ref="B24:B27"/>
@@ -2749,14 +2772,6 @@
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="B50:B54"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="B60:B64"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="B85:B89"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="B94:B98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2764,24 +2779,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>